<commit_message>
Fixed up/rewrote a few checks. Removed a visual bug in the tester where fails in the criterion were listed out of the number of passes e.g. Test: Criterion 3.3.2 Labels or Instructions-fail (6/4) passed when there were 4 pass tests and 6 fail tests
</commit_message>
<xml_diff>
--- a/erd.xlsx
+++ b/erd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\Documents\GDP14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC30437-AAD1-4397-9A0C-F40AECB3EEDF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3A492C-59C9-4091-AAB7-E2DB0A7C2A0B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{A21958E5-41B5-4DC6-A09B-B71F6B02FA63}"/>
   </bookViews>
@@ -494,7 +494,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Debugged some parts of the database interface, changed source to be a mediumblob instead of blob for more space to store source
</commit_message>
<xml_diff>
--- a/erd.xlsx
+++ b/erd.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\Documents\GDP14\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forth\Google Drive\Tom\UNIVERSITY\18_19 Computer Science\ELEC6200 - GDP\App ASUS\GDP14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3A492C-59C9-4091-AAB7-E2DB0A7C2A0B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{A21958E5-41B5-4DC6-A09B-B71F6B02FA63}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>page</t>
   </si>
@@ -108,12 +107,15 @@
   </si>
   <si>
     <t>eleTagNum</t>
+  </si>
+  <si>
+    <t>MEDIUMBLOB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -490,26 +492,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{713F9A80-2641-477B-994D-BEDD1493FBE1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -520,7 +522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -555,7 +557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>10000001</v>
       </c>
@@ -575,7 +577,7 @@
         <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="L3">
         <v>1000000001</v>
@@ -590,12 +592,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -621,7 +623,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1000000001</v>
       </c>
@@ -649,7 +651,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{33DEE1CE-3D5D-42C9-B6A8-5000453108F4}"/>
+    <hyperlink ref="B3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>